<commit_message>
fixed excel data from SQL
</commit_message>
<xml_diff>
--- a/covid_analysis/3_percentpopulationinfected.xlsx
+++ b/covid_analysis/3_percentpopulationinfected.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/User/Desktop/data_analysis_portfolio/covid_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{275C36F3-B018-FD4F-BACB-5F8A2BF2111B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43EEC6A6-B826-0A4E-968B-5DE377EF54F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="880" yWindow="1500" windowWidth="24640" windowHeight="13400" xr2:uid="{A8DDA2D5-0C43-C149-AB7B-802D111F7884}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$201</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="259">
   <si>
     <t>location</t>
   </si>
@@ -645,6 +648,171 @@
   </si>
   <si>
     <t>Zimbabwe</t>
+  </si>
+  <si>
+    <t>Lesotho</t>
+  </si>
+  <si>
+    <t>Djibouti</t>
+  </si>
+  <si>
+    <t>Mauritania</t>
+  </si>
+  <si>
+    <t>Bangladesh</t>
+  </si>
+  <si>
+    <t>Myanmar</t>
+  </si>
+  <si>
+    <t>Comoros</t>
+  </si>
+  <si>
+    <t>Equatorial Guinea</t>
+  </si>
+  <si>
+    <t>Rwanda</t>
+  </si>
+  <si>
+    <t>Cambodia</t>
+  </si>
+  <si>
+    <t>Uzbekistan</t>
+  </si>
+  <si>
+    <t>Africa</t>
+  </si>
+  <si>
+    <t>Mozambique</t>
+  </si>
+  <si>
+    <t>Pakistan</t>
+  </si>
+  <si>
+    <t>Kenya</t>
+  </si>
+  <si>
+    <t>Algeria</t>
+  </si>
+  <si>
+    <t>Senegal</t>
+  </si>
+  <si>
+    <t>Ghana</t>
+  </si>
+  <si>
+    <t>Afghanistan</t>
+  </si>
+  <si>
+    <t>Gambia</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>Papua New Guinea</t>
+  </si>
+  <si>
+    <t>Cameroon</t>
+  </si>
+  <si>
+    <t>Togo</t>
+  </si>
+  <si>
+    <t>Malawi</t>
+  </si>
+  <si>
+    <t>Guinea-Bissau</t>
+  </si>
+  <si>
+    <t>Congo</t>
+  </si>
+  <si>
+    <t>Burundi</t>
+  </si>
+  <si>
+    <t>Ethiopia</t>
+  </si>
+  <si>
+    <t>Uganda</t>
+  </si>
+  <si>
+    <t>Cote d'Ivoire</t>
+  </si>
+  <si>
+    <t>Low income</t>
+  </si>
+  <si>
+    <t>Angola</t>
+  </si>
+  <si>
+    <t>Haiti</t>
+  </si>
+  <si>
+    <t>Eritrea</t>
+  </si>
+  <si>
+    <t>Guinea</t>
+  </si>
+  <si>
+    <t>Central African Republic</t>
+  </si>
+  <si>
+    <t>Tokelau</t>
+  </si>
+  <si>
+    <t>Syria</t>
+  </si>
+  <si>
+    <t>Madagascar</t>
+  </si>
+  <si>
+    <t>Nicaragua</t>
+  </si>
+  <si>
+    <t>Benin</t>
+  </si>
+  <si>
+    <t>Tajikistan</t>
+  </si>
+  <si>
+    <t>South Sudan</t>
+  </si>
+  <si>
+    <t>Somalia</t>
+  </si>
+  <si>
+    <t>Liberia</t>
+  </si>
+  <si>
+    <t>Mali</t>
+  </si>
+  <si>
+    <t>Sudan</t>
+  </si>
+  <si>
+    <t>Nigeria</t>
+  </si>
+  <si>
+    <t>Burkina Faso</t>
+  </si>
+  <si>
+    <t>Democratic Republic of Congo</t>
+  </si>
+  <si>
+    <t>Sierra Leone</t>
+  </si>
+  <si>
+    <t>Tanzania</t>
+  </si>
+  <si>
+    <t>Chad</t>
+  </si>
+  <si>
+    <t>Niger</t>
+  </si>
+  <si>
+    <t>Yemen</t>
   </si>
 </sst>
 </file>
@@ -997,10 +1165,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA12B2A0-FCAE-8E4A-BEEB-E21B3BE2C7A1}">
-  <dimension ref="A1:D201"/>
+  <dimension ref="A1:D256"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3823,7 +3991,778 @@
         <v>1.6199893888000001</v>
       </c>
     </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>204</v>
+      </c>
+      <c r="B202" s="1">
+        <v>2305826</v>
+      </c>
+      <c r="C202" s="1">
+        <v>34490</v>
+      </c>
+      <c r="D202" s="1">
+        <v>1.4957763508999999</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>205</v>
+      </c>
+      <c r="B203" s="1">
+        <v>1120851</v>
+      </c>
+      <c r="C203" s="1">
+        <v>15690</v>
+      </c>
+      <c r="D203" s="1">
+        <v>1.3998292369000001</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>206</v>
+      </c>
+      <c r="B204" s="1">
+        <v>4736146</v>
+      </c>
+      <c r="C204" s="1">
+        <v>63439</v>
+      </c>
+      <c r="D204" s="1">
+        <v>1.3394646195</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
+        <v>207</v>
+      </c>
+      <c r="B205" s="1">
+        <v>171186368</v>
+      </c>
+      <c r="C205" s="1">
+        <v>2037947</v>
+      </c>
+      <c r="D205" s="1">
+        <v>1.1904843965</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>208</v>
+      </c>
+      <c r="B206" s="1">
+        <v>54179312</v>
+      </c>
+      <c r="C206" s="1">
+        <v>633967</v>
+      </c>
+      <c r="D206" s="1">
+        <v>1.1701274464</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>209</v>
+      </c>
+      <c r="B207" s="1">
+        <v>836783</v>
+      </c>
+      <c r="C207" s="1">
+        <v>9048</v>
+      </c>
+      <c r="D207" s="1">
+        <v>1.0812839170999999</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>210</v>
+      </c>
+      <c r="B208" s="1">
+        <v>1674916</v>
+      </c>
+      <c r="C208" s="1">
+        <v>17130</v>
+      </c>
+      <c r="D208" s="1">
+        <v>1.0227378567000001</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>211</v>
+      </c>
+      <c r="B209" s="1">
+        <v>13776702</v>
+      </c>
+      <c r="C209" s="1">
+        <v>133194</v>
+      </c>
+      <c r="D209" s="1">
+        <v>0.96680613400000004</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>214</v>
+      </c>
+      <c r="B210" s="1">
+        <v>1426736614</v>
+      </c>
+      <c r="C210" s="1">
+        <v>13063184</v>
+      </c>
+      <c r="D210" s="1">
+        <v>0.91559884790000001</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>212</v>
+      </c>
+      <c r="B211" s="1">
+        <v>16767851</v>
+      </c>
+      <c r="C211" s="1">
+        <v>138720</v>
+      </c>
+      <c r="D211" s="1">
+        <v>0.82729742770000003</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>213</v>
+      </c>
+      <c r="B212" s="1">
+        <v>34627648</v>
+      </c>
+      <c r="C212" s="1">
+        <v>251430</v>
+      </c>
+      <c r="D212" s="1">
+        <v>0.72609609519999996</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>215</v>
+      </c>
+      <c r="B213" s="1">
+        <v>32969520</v>
+      </c>
+      <c r="C213" s="1">
+        <v>233214</v>
+      </c>
+      <c r="D213" s="1">
+        <v>0.70736243659999998</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>216</v>
+      </c>
+      <c r="B214" s="1">
+        <v>235824864</v>
+      </c>
+      <c r="C214" s="1">
+        <v>1577699</v>
+      </c>
+      <c r="D214" s="1">
+        <v>0.66901300109999995</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>217</v>
+      </c>
+      <c r="B215" s="1">
+        <v>54027484</v>
+      </c>
+      <c r="C215" s="1">
+        <v>342943</v>
+      </c>
+      <c r="D215" s="1">
+        <v>0.63475656199999997</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>218</v>
+      </c>
+      <c r="B216" s="1">
+        <v>44903228</v>
+      </c>
+      <c r="C216" s="1">
+        <v>271522</v>
+      </c>
+      <c r="D216" s="1">
+        <v>0.60468258539999997</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A217" t="s">
+        <v>219</v>
+      </c>
+      <c r="B217" s="1">
+        <v>17316452</v>
+      </c>
+      <c r="C217" s="1">
+        <v>88933</v>
+      </c>
+      <c r="D217" s="1">
+        <v>0.51357518270000002</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A218" t="s">
+        <v>220</v>
+      </c>
+      <c r="B218" s="1">
+        <v>33475870</v>
+      </c>
+      <c r="C218" s="1">
+        <v>171281</v>
+      </c>
+      <c r="D218" s="1">
+        <v>0.51165511159999999</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
+        <v>221</v>
+      </c>
+      <c r="B219" s="1">
+        <v>41128772</v>
+      </c>
+      <c r="C219" s="1">
+        <v>209602</v>
+      </c>
+      <c r="D219" s="1">
+        <v>0.50962377380000001</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A220" t="s">
+        <v>222</v>
+      </c>
+      <c r="B220" s="1">
+        <v>2705995</v>
+      </c>
+      <c r="C220" s="1">
+        <v>12598</v>
+      </c>
+      <c r="D220" s="1">
+        <v>0.46555887950000002</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A221" t="s">
+        <v>223</v>
+      </c>
+      <c r="B221" s="1">
+        <v>110990096</v>
+      </c>
+      <c r="C221" s="1">
+        <v>515792</v>
+      </c>
+      <c r="D221" s="1">
+        <v>0.46471894209999998</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A222" t="s">
+        <v>224</v>
+      </c>
+      <c r="B222" s="1">
+        <v>10142625</v>
+      </c>
+      <c r="C222" s="1">
+        <v>46826</v>
+      </c>
+      <c r="D222" s="1">
+        <v>0.46167535520000003</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A223" t="s">
+        <v>225</v>
+      </c>
+      <c r="B223" s="1">
+        <v>27914542</v>
+      </c>
+      <c r="C223" s="1">
+        <v>124605</v>
+      </c>
+      <c r="D223" s="1">
+        <v>0.4463802415</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A224" t="s">
+        <v>226</v>
+      </c>
+      <c r="B224" s="1">
+        <v>8848700</v>
+      </c>
+      <c r="C224" s="1">
+        <v>39407</v>
+      </c>
+      <c r="D224" s="1">
+        <v>0.44534225370000002</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A225" t="s">
+        <v>227</v>
+      </c>
+      <c r="B225" s="1">
+        <v>20405318</v>
+      </c>
+      <c r="C225" s="1">
+        <v>88613</v>
+      </c>
+      <c r="D225" s="1">
+        <v>0.43426424429999999</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A226" t="s">
+        <v>228</v>
+      </c>
+      <c r="B226" s="1">
+        <v>2105580</v>
+      </c>
+      <c r="C226" s="1">
+        <v>8960</v>
+      </c>
+      <c r="D226" s="1">
+        <v>0.4255359568</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A227" t="s">
+        <v>229</v>
+      </c>
+      <c r="B227" s="1">
+        <v>5970430</v>
+      </c>
+      <c r="C227" s="1">
+        <v>25110</v>
+      </c>
+      <c r="D227" s="1">
+        <v>0.4205727226</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A228" t="s">
+        <v>230</v>
+      </c>
+      <c r="B228" s="1">
+        <v>12889583</v>
+      </c>
+      <c r="C228" s="1">
+        <v>53661</v>
+      </c>
+      <c r="D228" s="1">
+        <v>0.41631292489999999</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A229" t="s">
+        <v>231</v>
+      </c>
+      <c r="B229" s="1">
+        <v>123379928</v>
+      </c>
+      <c r="C229" s="1">
+        <v>500169</v>
+      </c>
+      <c r="D229" s="1">
+        <v>0.40538927860000001</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A230" t="s">
+        <v>232</v>
+      </c>
+      <c r="B230" s="1">
+        <v>47249588</v>
+      </c>
+      <c r="C230" s="1">
+        <v>170463</v>
+      </c>
+      <c r="D230" s="1">
+        <v>0.3607713997</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A231" t="s">
+        <v>233</v>
+      </c>
+      <c r="B231" s="1">
+        <v>28160548</v>
+      </c>
+      <c r="C231" s="1">
+        <v>88277</v>
+      </c>
+      <c r="D231" s="1">
+        <v>0.31347756440000002</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A232" t="s">
+        <v>234</v>
+      </c>
+      <c r="B232" s="1">
+        <v>737604900</v>
+      </c>
+      <c r="C232" s="1">
+        <v>2287803</v>
+      </c>
+      <c r="D232" s="1">
+        <v>0.31016645900000001</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A233" t="s">
+        <v>235</v>
+      </c>
+      <c r="B233" s="1">
+        <v>35588996</v>
+      </c>
+      <c r="C233" s="1">
+        <v>105298</v>
+      </c>
+      <c r="D233" s="1">
+        <v>0.29587235340000001</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A234" t="s">
+        <v>236</v>
+      </c>
+      <c r="B234" s="1">
+        <v>11585003</v>
+      </c>
+      <c r="C234" s="1">
+        <v>34202</v>
+      </c>
+      <c r="D234" s="1">
+        <v>0.29522650969999997</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A235" t="s">
+        <v>237</v>
+      </c>
+      <c r="B235" s="1">
+        <v>3684041</v>
+      </c>
+      <c r="C235" s="1">
+        <v>10189</v>
+      </c>
+      <c r="D235" s="1">
+        <v>0.2765712977</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A236" t="s">
+        <v>238</v>
+      </c>
+      <c r="B236" s="1">
+        <v>13859349</v>
+      </c>
+      <c r="C236" s="1">
+        <v>38280</v>
+      </c>
+      <c r="D236" s="1">
+        <v>0.27620344940000002</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A237" t="s">
+        <v>239</v>
+      </c>
+      <c r="B237" s="1">
+        <v>5579148</v>
+      </c>
+      <c r="C237" s="1">
+        <v>15367</v>
+      </c>
+      <c r="D237" s="1">
+        <v>0.27543632109999999</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A238" t="s">
+        <v>240</v>
+      </c>
+      <c r="B238" s="1">
+        <v>1893</v>
+      </c>
+      <c r="C238" s="1">
+        <v>5</v>
+      </c>
+      <c r="D238" s="1">
+        <v>0.26413100900000003</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A239" t="s">
+        <v>241</v>
+      </c>
+      <c r="B239" s="1">
+        <v>22125242</v>
+      </c>
+      <c r="C239" s="1">
+        <v>57423</v>
+      </c>
+      <c r="D239" s="1">
+        <v>0.25953614429999999</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A240" t="s">
+        <v>242</v>
+      </c>
+      <c r="B240" s="1">
+        <v>29611718</v>
+      </c>
+      <c r="C240" s="1">
+        <v>67941</v>
+      </c>
+      <c r="D240" s="1">
+        <v>0.2294395752</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A241" t="s">
+        <v>243</v>
+      </c>
+      <c r="B241" s="1">
+        <v>6948395</v>
+      </c>
+      <c r="C241" s="1">
+        <v>15672</v>
+      </c>
+      <c r="D241" s="1">
+        <v>0.22554848999999999</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A242" t="s">
+        <v>244</v>
+      </c>
+      <c r="B242" s="1">
+        <v>13352864</v>
+      </c>
+      <c r="C242" s="1">
+        <v>27999</v>
+      </c>
+      <c r="D242" s="1">
+        <v>0.20968535290000001</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A243" t="s">
+        <v>245</v>
+      </c>
+      <c r="B243" s="1">
+        <v>9952789</v>
+      </c>
+      <c r="C243" s="1">
+        <v>17786</v>
+      </c>
+      <c r="D243" s="1">
+        <v>0.1787036779</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A244" t="s">
+        <v>246</v>
+      </c>
+      <c r="B244" s="1">
+        <v>10913172</v>
+      </c>
+      <c r="C244" s="1">
+        <v>18368</v>
+      </c>
+      <c r="D244" s="1">
+        <v>0.16831036839999999</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A245" t="s">
+        <v>247</v>
+      </c>
+      <c r="B245" s="1">
+        <v>17597508</v>
+      </c>
+      <c r="C245" s="1">
+        <v>27324</v>
+      </c>
+      <c r="D245" s="1">
+        <v>0.15527198510000001</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A246" t="s">
+        <v>248</v>
+      </c>
+      <c r="B246" s="1">
+        <v>5302690</v>
+      </c>
+      <c r="C246" s="1">
+        <v>8090</v>
+      </c>
+      <c r="D246" s="1">
+        <v>0.15256407599999999</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A247" t="s">
+        <v>249</v>
+      </c>
+      <c r="B247" s="1">
+        <v>22593598</v>
+      </c>
+      <c r="C247" s="1">
+        <v>33067</v>
+      </c>
+      <c r="D247" s="1">
+        <v>0.1463556181</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A248" t="s">
+        <v>250</v>
+      </c>
+      <c r="B248" s="1">
+        <v>46874200</v>
+      </c>
+      <c r="C248" s="1">
+        <v>63853</v>
+      </c>
+      <c r="D248" s="1">
+        <v>0.1362220582</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A249" t="s">
+        <v>251</v>
+      </c>
+      <c r="B249" s="1">
+        <v>218541216</v>
+      </c>
+      <c r="C249" s="1">
+        <v>266641</v>
+      </c>
+      <c r="D249" s="1">
+        <v>0.1220094794</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A250" t="s">
+        <v>252</v>
+      </c>
+      <c r="B250" s="1">
+        <v>22673764</v>
+      </c>
+      <c r="C250" s="1">
+        <v>22056</v>
+      </c>
+      <c r="D250" s="1">
+        <v>9.7275423700000002E-2</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A251" t="s">
+        <v>253</v>
+      </c>
+      <c r="B251" s="1">
+        <v>99010216</v>
+      </c>
+      <c r="C251" s="1">
+        <v>95814</v>
+      </c>
+      <c r="D251" s="1">
+        <v>9.6771832099999996E-2</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A252" t="s">
+        <v>254</v>
+      </c>
+      <c r="B252" s="1">
+        <v>8605723</v>
+      </c>
+      <c r="C252" s="1">
+        <v>7760</v>
+      </c>
+      <c r="D252" s="1">
+        <v>9.0172551500000003E-2</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A253" t="s">
+        <v>255</v>
+      </c>
+      <c r="B253" s="1">
+        <v>65497752</v>
+      </c>
+      <c r="C253" s="1">
+        <v>42927</v>
+      </c>
+      <c r="D253" s="1">
+        <v>6.5539653899999994E-2</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A254" t="s">
+        <v>256</v>
+      </c>
+      <c r="B254" s="1">
+        <v>17723312</v>
+      </c>
+      <c r="C254" s="1">
+        <v>7682</v>
+      </c>
+      <c r="D254" s="1">
+        <v>4.33440431E-2</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A255" t="s">
+        <v>257</v>
+      </c>
+      <c r="B255" s="1">
+        <v>26207982</v>
+      </c>
+      <c r="C255" s="1">
+        <v>9513</v>
+      </c>
+      <c r="D255" s="1">
+        <v>3.6298101899999997E-2</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A256" t="s">
+        <v>258</v>
+      </c>
+      <c r="B256" s="1">
+        <v>33696612</v>
+      </c>
+      <c r="C256" s="1">
+        <v>11945</v>
+      </c>
+      <c r="D256" s="1">
+        <v>3.5448667699999999E-2</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:D201" xr:uid="{CA12B2A0-FCAE-8E4A-BEEB-E21B3BE2C7A1}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>